<commit_message>
added convergence criteria for MCS and done sime fixes
</commit_message>
<xml_diff>
--- a/MonteCarloResultsRBMCp214.xlsx
+++ b/MonteCarloResultsRBMCp214.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Customer type</t>
   </si>
@@ -50,6 +50,15 @@
   </si>
   <si>
     <t>EENS</t>
+  </si>
+  <si>
+    <t>nr of simulations</t>
+  </si>
+  <si>
+    <t>provided beta</t>
+  </si>
+  <si>
+    <t>calculated beta</t>
   </si>
   <si>
     <t>A</t>
@@ -422,13 +431,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:16">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,13 +474,22 @@
       <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <v>0.535</v>
@@ -483,36 +501,36 @@
         <v>210</v>
       </c>
       <c r="F2">
-        <v>352.3518559803952</v>
+        <v>-1.627534966661221</v>
       </c>
       <c r="G2">
-        <v>592</v>
+        <v>811</v>
       </c>
       <c r="H2">
-        <v>1.19037789182566</v>
+        <v>1.188040320916699</v>
       </c>
       <c r="I2">
-        <v>296</v>
+        <v>-1.369932432432432</v>
       </c>
       <c r="J2">
-        <v>62160</v>
+        <v>-287.6858108108108</v>
       </c>
       <c r="K2">
-        <v>73993.88975588299</v>
+        <v>-341.7823429988565</v>
       </c>
       <c r="L2">
-        <v>249.9793572833885</v>
+        <v>249.4884673925068</v>
       </c>
       <c r="M2">
-        <v>188.5082429495114</v>
+        <v>-0.8707312071637534</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>0.535</v>
@@ -524,36 +542,36 @@
         <v>210</v>
       </c>
       <c r="F3">
-        <v>408.9188991018648</v>
+        <v>-1.761145907544019</v>
       </c>
       <c r="G3">
-        <v>511</v>
+        <v>674</v>
       </c>
       <c r="H3">
-        <v>1.600465358520019</v>
+        <v>1.54688186537991</v>
       </c>
       <c r="I3">
-        <v>255.5</v>
+        <v>-1.138513513513514</v>
       </c>
       <c r="J3">
-        <v>53655</v>
+        <v>-239.0878378378379</v>
       </c>
       <c r="K3">
-        <v>85872.96881139162</v>
+        <v>-369.8406405842441</v>
       </c>
       <c r="L3">
-        <v>336.097725289204</v>
+        <v>324.8451917297811</v>
       </c>
       <c r="M3">
-        <v>218.7716110194977</v>
+        <v>-0.9422130605360505</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:16">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>0.535</v>
@@ -565,33 +583,33 @@
         <v>210</v>
       </c>
       <c r="F4">
-        <v>238.6448162702488</v>
+        <v>-1.068375785164082</v>
       </c>
       <c r="G4">
-        <v>370</v>
+        <v>507</v>
       </c>
       <c r="H4">
-        <v>1.289971979839183</v>
+        <v>1.247492041059441</v>
       </c>
       <c r="I4">
-        <v>185</v>
+        <v>-0.856418918918919</v>
       </c>
       <c r="J4">
-        <v>38850</v>
+        <v>-179.847972972973</v>
       </c>
       <c r="K4">
-        <v>50115.41141675224</v>
+        <v>-224.3589148844573</v>
       </c>
       <c r="L4">
-        <v>270.8941157662284</v>
+        <v>261.9733286224827</v>
       </c>
       <c r="M4">
-        <v>127.6749767045831</v>
+        <v>-0.5715810450627841</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:16">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>1.605</v>
@@ -603,16 +621,25 @@
         <v>630</v>
       </c>
       <c r="J5">
-        <v>245.5</v>
+        <v>-1.121621621621622</v>
       </c>
       <c r="K5">
-        <v>333.3051904508363</v>
+        <v>-1.485685553123108</v>
       </c>
       <c r="L5">
-        <v>1.357658616907683</v>
+        <v>1.324587119651927</v>
       </c>
       <c r="M5">
-        <v>534.9548306735923</v>
+        <v>-2.384525312762588</v>
+      </c>
+      <c r="N5">
+        <v>8</v>
+      </c>
+      <c r="O5">
+        <v>0.02</v>
+      </c>
+      <c r="P5">
+        <v>0.001867481408371164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>